<commit_message>
Correção do código de avaliação de redução de etapas in vivo
</commit_message>
<xml_diff>
--- a/validacao/validacao_rat_vi_nova_predicao.xlsx
+++ b/validacao/validacao_rat_vi_nova_predicao.xlsx
@@ -940,7 +940,7 @@
         <v>0</v>
       </c>
       <c r="H19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1798,7 +1798,7 @@
         <v>0</v>
       </c>
       <c r="H52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -3592,7 +3592,7 @@
         <v>0</v>
       </c>
       <c r="H121" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122">
@@ -4684,7 +4684,7 @@
         <v>0</v>
       </c>
       <c r="H163" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164">
@@ -5048,7 +5048,7 @@
         <v>0</v>
       </c>
       <c r="H177" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178">
@@ -5334,7 +5334,7 @@
         <v>0</v>
       </c>
       <c r="H188" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189">
@@ -7518,7 +7518,7 @@
         <v>0</v>
       </c>
       <c r="H272" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="273">
@@ -12380,7 +12380,7 @@
         <v>0</v>
       </c>
       <c r="H459" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="460">
@@ -12744,7 +12744,7 @@
         <v>0</v>
       </c>
       <c r="H473" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="474">
@@ -14486,7 +14486,7 @@
         <v>0</v>
       </c>
       <c r="H540" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="541">

</xml_diff>